<commit_message>
everything works. cleanup needed
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -131,7 +131,7 @@
     <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
   </si>
   <si>
-    <t>who is going to die</t>
+    <t>Меню</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -486,7 +486,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="4">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1">

</xml_diff>

<commit_message>
healthchecks added && readme updated
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -556,7 +556,7 @@
     <col min="6" max="6" style="15" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -570,7 +570,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1"/>
       <c r="B2" s="5">
         <v>3</v>
@@ -584,7 +584,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5">
@@ -600,7 +600,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="5">
@@ -616,7 +616,7 @@
         <v>215.36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="32.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5">
@@ -632,7 +632,7 @@
         <v>265.57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1"/>
       <c r="B6" s="5">
         <v>4</v>
@@ -646,7 +646,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="32.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5">
@@ -662,7 +662,7 @@
         <v>166.47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="32.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="5">
@@ -678,7 +678,7 @@
         <v>168.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="46.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="45">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5">
@@ -694,7 +694,7 @@
         <v>132.88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -708,7 +708,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1"/>
       <c r="B11" s="5">
         <v>5</v>
@@ -722,7 +722,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5">
@@ -738,7 +738,7 @@
         <v>2700.79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5">
@@ -754,7 +754,7 @@
         <v>3100.33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="5">
@@ -770,7 +770,7 @@
         <v>1850.42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1"/>
       <c r="B15" s="5">
         <v>6</v>
@@ -784,7 +784,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="32.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="5">
@@ -800,7 +800,7 @@
         <v>420.78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="32.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="5">
@@ -816,7 +816,7 @@
         <v>440.11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="47.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="45.75">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="5">
@@ -832,7 +832,7 @@
         <v>520.08</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -840,7 +840,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -848,7 +848,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -856,7 +856,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -864,7 +864,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -872,7 +872,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -880,7 +880,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -888,7 +888,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -896,7 +896,7 @@
       <c r="E26" s="10"/>
       <c r="F26" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -904,7 +904,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -912,7 +912,7 @@
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -920,7 +920,7 @@
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -928,7 +928,7 @@
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -936,7 +936,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>

</xml_diff>